<commit_message>
Adding name to rubric
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C315C46E-72F2-490B-A085-C11E3622EA94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D8EE78-3AB9-43DE-85ED-88C0A0E1F1E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -335,7 +335,7 @@
     <t xml:space="preserve">Full FPS Style flythrough camera [see end of day 3 slides]. </t>
   </si>
   <si>
-    <t>Student Names: Julio Delgado</t>
+    <t>Student Names: Julio Delgado, Travis Jaczewski</t>
   </si>
 </sst>
 </file>
@@ -937,21 +937,21 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="106.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="106.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="6" width="25.44140625" customWidth="1"/>
-    <col min="7" max="7" width="25.5546875" customWidth="1"/>
-    <col min="8" max="9" width="25.88671875" customWidth="1"/>
-    <col min="10" max="10" width="24.5546875" customWidth="1"/>
-    <col min="11" max="11" width="24.44140625" customWidth="1"/>
-    <col min="12" max="12" width="24.109375" customWidth="1"/>
-    <col min="13" max="14" width="9.109375" customWidth="1"/>
+    <col min="4" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" customWidth="1"/>
+    <col min="8" max="9" width="25.85546875" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>101</v>
       </c>
@@ -967,7 +967,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>28</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>97</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>93</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>72</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>39</v>
       </c>
@@ -1176,7 +1176,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>40</v>
       </c>
@@ -1210,7 +1210,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>41</v>
       </c>
@@ -1241,7 +1241,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>42</v>
       </c>
@@ -1275,7 +1275,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>50</v>
       </c>
@@ -1300,7 +1300,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>57</v>
       </c>
@@ -1325,7 +1325,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>75</v>
       </c>
@@ -1350,7 +1350,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>76</v>
       </c>
@@ -1375,7 +1375,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>46</v>
       </c>
@@ -1400,7 +1400,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1417,7 +1417,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>52</v>
       </c>
@@ -1436,7 +1436,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1453,7 +1453,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1470,7 +1470,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>9</v>
       </c>
@@ -1489,7 +1489,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>37</v>
       </c>
@@ -1514,7 +1514,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
@@ -1539,7 +1539,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>38</v>
       </c>
@@ -1564,7 +1564,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>36</v>
       </c>
@@ -1589,7 +1589,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>77</v>
       </c>
@@ -1614,7 +1614,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1631,7 +1631,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>73</v>
       </c>
@@ -1650,7 +1650,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>78</v>
       </c>
@@ -1675,7 +1675,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>65</v>
       </c>
@@ -1700,7 +1700,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>67</v>
       </c>
@@ -1725,7 +1725,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>66</v>
       </c>
@@ -1750,7 +1750,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>68</v>
       </c>
@@ -1775,7 +1775,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>69</v>
       </c>
@@ -1800,7 +1800,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1817,7 +1817,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1834,7 +1834,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>53</v>
       </c>
@@ -1853,7 +1853,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>98</v>
       </c>
@@ -1878,7 +1878,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>79</v>
       </c>
@@ -1903,7 +1903,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>94</v>
       </c>
@@ -1928,7 +1928,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>92</v>
       </c>
@@ -1953,7 +1953,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>45</v>
       </c>
@@ -1978,7 +1978,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>33</v>
       </c>
@@ -2003,7 +2003,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>34</v>
       </c>
@@ -2028,7 +2028,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>54</v>
       </c>
@@ -2053,7 +2053,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>35</v>
       </c>
@@ -2078,7 +2078,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>70</v>
       </c>
@@ -2103,7 +2103,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2120,7 +2120,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2137,7 +2137,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>7</v>
       </c>
@@ -2156,7 +2156,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>74</v>
       </c>
@@ -2181,7 +2181,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>47</v>
       </c>
@@ -2206,7 +2206,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>55</v>
       </c>
@@ -2231,7 +2231,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>71</v>
       </c>
@@ -2256,7 +2256,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2273,7 +2273,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>6</v>
       </c>
@@ -2292,7 +2292,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>80</v>
       </c>
@@ -2317,7 +2317,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>64</v>
       </c>
@@ -2342,7 +2342,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>99</v>
       </c>
@@ -2367,7 +2367,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>48</v>
       </c>
@@ -2392,7 +2392,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2409,7 +2409,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2426,7 +2426,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>5</v>
       </c>
@@ -2445,7 +2445,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
         <v>100</v>
       </c>
@@ -2470,7 +2470,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
         <v>95</v>
       </c>
@@ -2495,7 +2495,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
         <v>82</v>
       </c>
@@ -2520,7 +2520,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
         <v>58</v>
       </c>
@@ -2545,7 +2545,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
         <v>56</v>
       </c>
@@ -2570,7 +2570,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>49</v>
       </c>
@@ -2595,7 +2595,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2612,7 +2612,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2629,7 +2629,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>4</v>
       </c>
@@ -2648,7 +2648,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>85</v>
       </c>
@@ -2673,7 +2673,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>91</v>
       </c>
@@ -2698,7 +2698,7 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>86</v>
       </c>
@@ -2723,7 +2723,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>88</v>
       </c>
@@ -2748,7 +2748,7 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>87</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>89</v>
       </c>
@@ -2798,7 +2798,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>90</v>
       </c>
@@ -2823,7 +2823,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
@@ -2840,7 +2840,7 @@
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
@@ -2857,7 +2857,7 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>84</v>
       </c>
@@ -2876,7 +2876,7 @@
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>62</v>
       </c>
@@ -2897,7 +2897,7 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>63</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
         <v>83</v>
       </c>
@@ -2939,7 +2939,7 @@
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
         <v>60</v>
       </c>
@@ -2960,7 +2960,7 @@
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>59</v>
       </c>
@@ -2981,7 +2981,7 @@
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>61</v>
       </c>
@@ -3002,7 +3002,7 @@
       <c r="K87" s="5"/>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3019,7 +3019,7 @@
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3036,7 +3036,7 @@
       <c r="K89" s="5"/>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>31</v>
       </c>
@@ -3060,7 +3060,7 @@
       <c r="K90" s="6"/>
       <c r="L90" s="5"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
         <v>17</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="K91" s="6"/>
       <c r="L91" s="5"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>29</v>
       </c>
@@ -3096,7 +3096,7 @@
       <c r="K92" s="6"/>
       <c r="L92" s="5"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="11"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -3110,7 +3110,7 @@
       <c r="K93" s="6"/>
       <c r="L93" s="5"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="11"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
@@ -3124,78 +3124,78 @@
       <c r="K94" s="5"/>
       <c r="L94" s="5"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="12"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="13"/>
     </row>
   </sheetData>
@@ -3220,7 +3220,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3290,7 +3290,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3307,7 +3307,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Add Angel to rubric Add Template files
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D8EE78-3AB9-43DE-85ED-88C0A0E1F1E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BFF6C1-4472-4C66-99C7-DFDF9C82CF95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -335,7 +335,7 @@
     <t xml:space="preserve">Full FPS Style flythrough camera [see end of day 3 slides]. </t>
   </si>
   <si>
-    <t>Student Names: Julio Delgado, Travis Jaczewski</t>
+    <t>Student Names: Julio Delgado, Travis Jaczewski, Angel Rivera Velez</t>
   </si>
 </sst>
 </file>
@@ -937,21 +937,21 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="106.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="106.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1"/>
-    <col min="8" max="9" width="25.85546875" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" customWidth="1"/>
+    <col min="4" max="6" width="25.44140625" customWidth="1"/>
+    <col min="7" max="7" width="25.5546875" customWidth="1"/>
+    <col min="8" max="9" width="25.88671875" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" customWidth="1"/>
+    <col min="11" max="11" width="24.44140625" customWidth="1"/>
+    <col min="12" max="12" width="24.109375" customWidth="1"/>
+    <col min="13" max="14" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>101</v>
       </c>
@@ -967,7 +967,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>28</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>97</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>93</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>72</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>39</v>
       </c>
@@ -1176,7 +1176,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>40</v>
       </c>
@@ -1210,7 +1210,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>41</v>
       </c>
@@ -1241,7 +1241,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>42</v>
       </c>
@@ -1275,7 +1275,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>50</v>
       </c>
@@ -1300,7 +1300,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>57</v>
       </c>
@@ -1325,7 +1325,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>75</v>
       </c>
@@ -1350,7 +1350,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>76</v>
       </c>
@@ -1375,7 +1375,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>46</v>
       </c>
@@ -1400,7 +1400,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1417,7 +1417,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>52</v>
       </c>
@@ -1436,7 +1436,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1453,7 +1453,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1470,7 +1470,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>9</v>
       </c>
@@ -1489,7 +1489,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>37</v>
       </c>
@@ -1514,7 +1514,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
@@ -1539,7 +1539,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>38</v>
       </c>
@@ -1564,7 +1564,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>36</v>
       </c>
@@ -1589,7 +1589,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>77</v>
       </c>
@@ -1614,7 +1614,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1631,7 +1631,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>73</v>
       </c>
@@ -1650,7 +1650,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>78</v>
       </c>
@@ -1675,7 +1675,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>65</v>
       </c>
@@ -1700,7 +1700,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>67</v>
       </c>
@@ -1725,7 +1725,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>66</v>
       </c>
@@ -1750,7 +1750,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>68</v>
       </c>
@@ -1775,7 +1775,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>69</v>
       </c>
@@ -1800,7 +1800,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1817,7 +1817,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1834,7 +1834,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>53</v>
       </c>
@@ -1853,7 +1853,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
         <v>98</v>
       </c>
@@ -1878,7 +1878,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="24" t="s">
         <v>79</v>
       </c>
@@ -1903,7 +1903,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>94</v>
       </c>
@@ -1928,7 +1928,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>92</v>
       </c>
@@ -1953,7 +1953,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>45</v>
       </c>
@@ -1978,7 +1978,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>33</v>
       </c>
@@ -2003,7 +2003,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>34</v>
       </c>
@@ -2028,7 +2028,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>54</v>
       </c>
@@ -2053,7 +2053,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>35</v>
       </c>
@@ -2078,7 +2078,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
         <v>70</v>
       </c>
@@ -2103,7 +2103,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="22"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2120,7 +2120,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2137,7 +2137,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>7</v>
       </c>
@@ -2156,7 +2156,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
         <v>74</v>
       </c>
@@ -2181,7 +2181,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>47</v>
       </c>
@@ -2206,7 +2206,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>55</v>
       </c>
@@ -2231,7 +2231,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>71</v>
       </c>
@@ -2256,7 +2256,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="8"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2273,7 +2273,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
         <v>6</v>
       </c>
@@ -2292,7 +2292,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>80</v>
       </c>
@@ -2317,7 +2317,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>64</v>
       </c>
@@ -2342,7 +2342,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
         <v>99</v>
       </c>
@@ -2367,7 +2367,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>48</v>
       </c>
@@ -2392,7 +2392,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="8"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2409,7 +2409,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="8"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2426,7 +2426,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>5</v>
       </c>
@@ -2445,7 +2445,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>100</v>
       </c>
@@ -2470,7 +2470,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
         <v>95</v>
       </c>
@@ -2495,7 +2495,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
         <v>82</v>
       </c>
@@ -2520,7 +2520,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="20" t="s">
         <v>58</v>
       </c>
@@ -2545,7 +2545,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="21" t="s">
         <v>56</v>
       </c>
@@ -2570,7 +2570,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
         <v>49</v>
       </c>
@@ -2595,7 +2595,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="8"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2612,7 +2612,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="8"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2629,7 +2629,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>4</v>
       </c>
@@ -2648,7 +2648,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
         <v>85</v>
       </c>
@@ -2673,7 +2673,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
         <v>91</v>
       </c>
@@ -2698,7 +2698,7 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
         <v>86</v>
       </c>
@@ -2723,7 +2723,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
         <v>88</v>
       </c>
@@ -2748,7 +2748,7 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
         <v>87</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
         <v>89</v>
       </c>
@@ -2798,7 +2798,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
         <v>90</v>
       </c>
@@ -2823,7 +2823,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="11"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
@@ -2840,7 +2840,7 @@
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="11"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
@@ -2857,7 +2857,7 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
         <v>84</v>
       </c>
@@ -2876,7 +2876,7 @@
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
         <v>62</v>
       </c>
@@ -2897,7 +2897,7 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
         <v>63</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="11" t="s">
         <v>83</v>
       </c>
@@ -2939,7 +2939,7 @@
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="11" t="s">
         <v>60</v>
       </c>
@@ -2960,7 +2960,7 @@
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="11" t="s">
         <v>59</v>
       </c>
@@ -2981,7 +2981,7 @@
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="11" t="s">
         <v>61</v>
       </c>
@@ -3002,7 +3002,7 @@
       <c r="K87" s="5"/>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="8"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3019,7 +3019,7 @@
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="8"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3036,7 +3036,7 @@
       <c r="K89" s="5"/>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
         <v>31</v>
       </c>
@@ -3060,7 +3060,7 @@
       <c r="K90" s="6"/>
       <c r="L90" s="5"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="10" t="s">
         <v>17</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="K91" s="6"/>
       <c r="L91" s="5"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
         <v>29</v>
       </c>
@@ -3096,7 +3096,7 @@
       <c r="K92" s="6"/>
       <c r="L92" s="5"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="11"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -3110,7 +3110,7 @@
       <c r="K93" s="6"/>
       <c r="L93" s="5"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="11"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
@@ -3124,78 +3124,78 @@
       <c r="K94" s="5"/>
       <c r="L94" s="5"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="12"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="12"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="12"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="12"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="12"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="12"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="12"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="12"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="12"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="12"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="12"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="12"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="12"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="12"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="12"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="12"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="12"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="12"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="12"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="12"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="12"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="12"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="13"/>
     </row>
   </sheetData>
@@ -3220,7 +3220,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3290,7 +3290,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3307,7 +3307,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Add repo address into rubric
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BFF6C1-4472-4C66-99C7-DFDF9C82CF95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E47FDF5-8DA1-4321-ACEB-A793BE84B4D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,9 +116,6 @@
     <t>Before Carry</t>
   </si>
   <si>
-    <t>Student Git Address:</t>
-  </si>
-  <si>
     <t>All Graphics API Objects cleaned up in memory</t>
   </si>
   <si>
@@ -336,6 +333,9 @@
   </si>
   <si>
     <t>Student Names: Julio Delgado, Travis Jaczewski, Angel Rivera Velez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student Git Address: https://github.com/JulDel158/PPIV-Project.git </t>
   </si>
 </sst>
 </file>
@@ -935,7 +935,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -953,7 +955,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -969,7 +971,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -984,7 +986,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -1016,10 +1018,10 @@
         <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>27</v>
@@ -1032,12 +1034,12 @@
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="5">
         <v>4</v>
@@ -1077,7 +1079,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="5">
         <v>4</v>
@@ -1105,12 +1107,12 @@
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="5">
         <v>4</v>
@@ -1147,7 +1149,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -1178,7 +1180,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -1212,7 +1214,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
@@ -1243,7 +1245,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
@@ -1277,7 +1279,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="5">
         <v>2</v>
@@ -1302,7 +1304,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="5">
         <v>4</v>
@@ -1327,7 +1329,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -1352,7 +1354,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="5">
         <v>4</v>
@@ -1377,7 +1379,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="5">
         <v>2</v>
@@ -1419,7 +1421,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1491,7 +1493,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="5">
         <v>4</v>
@@ -1516,7 +1518,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="5">
         <v>2</v>
@@ -1541,7 +1543,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="5">
         <v>4</v>
@@ -1566,7 +1568,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="5">
         <v>3</v>
@@ -1591,7 +1593,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="5">
         <v>2</v>
@@ -1633,7 +1635,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1652,7 +1654,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="5">
         <v>3</v>
@@ -1677,7 +1679,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="5">
         <v>1</v>
@@ -1702,7 +1704,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" s="5">
         <v>3</v>
@@ -1727,7 +1729,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" s="5">
         <v>4</v>
@@ -1752,7 +1754,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B32" s="5">
         <v>2</v>
@@ -1777,7 +1779,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" s="5">
         <v>3</v>
@@ -1836,7 +1838,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1855,7 +1857,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B37" s="5">
         <v>3</v>
@@ -1880,7 +1882,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B38" s="5">
         <v>2</v>
@@ -1905,7 +1907,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B39" s="5">
         <v>4</v>
@@ -1930,7 +1932,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B40" s="5">
         <v>4</v>
@@ -1955,7 +1957,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" s="5">
         <v>4</v>
@@ -1980,7 +1982,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="5">
         <v>4</v>
@@ -2005,7 +2007,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B43" s="5">
         <v>1</v>
@@ -2030,7 +2032,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44" s="5">
         <v>1</v>
@@ -2055,7 +2057,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B45" s="5">
         <v>1</v>
@@ -2080,7 +2082,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B46" s="1">
         <v>3</v>
@@ -2158,7 +2160,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B50" s="5">
         <v>3</v>
@@ -2183,7 +2185,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B51" s="5">
         <v>4</v>
@@ -2208,7 +2210,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" s="5">
         <v>4</v>
@@ -2233,7 +2235,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B53" s="5">
         <v>4</v>
@@ -2294,7 +2296,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B56" s="5">
         <v>2</v>
@@ -2319,7 +2321,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B57" s="5">
         <v>2</v>
@@ -2344,7 +2346,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B58" s="5">
         <v>3</v>
@@ -2369,7 +2371,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B59" s="5">
         <v>4</v>
@@ -2447,7 +2449,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B63" s="5">
         <v>2</v>
@@ -2472,7 +2474,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B64" s="5">
         <v>1</v>
@@ -2497,7 +2499,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B65" s="5">
         <v>1</v>
@@ -2522,7 +2524,7 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B66" s="5">
         <v>1</v>
@@ -2547,7 +2549,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B67" s="5">
         <v>4</v>
@@ -2572,7 +2574,7 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B68" s="5">
         <v>4</v>
@@ -2650,7 +2652,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B72" s="5">
         <v>2</v>
@@ -2675,7 +2677,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B73" s="5">
         <v>1</v>
@@ -2700,7 +2702,7 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B74" s="5">
         <v>2</v>
@@ -2725,7 +2727,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B75" s="5">
         <v>3</v>
@@ -2750,7 +2752,7 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B76" s="5">
         <v>2</v>
@@ -2775,7 +2777,7 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B77" s="5">
         <v>3</v>
@@ -2800,7 +2802,7 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B78" s="5">
         <v>3</v>
@@ -2859,7 +2861,7 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
@@ -2878,7 +2880,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
@@ -2899,7 +2901,7 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
@@ -2920,7 +2922,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
@@ -2941,7 +2943,7 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
@@ -2962,7 +2964,7 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -2983,7 +2985,7 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -3038,7 +3040,7 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>18</v>
@@ -3080,7 +3082,7 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B92" s="6">
         <v>1</v>
@@ -3126,7 +3128,7 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
@@ -3220,7 +3222,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Add Renderable.h to project (work in progress) Add cleanup function in main.cpp marked row 37 as completed in rubric
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E47FDF5-8DA1-4321-ACEB-A793BE84B4D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25E3DD7-A948-4A89-A3AE-CB61D9988ADB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="103">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t xml:space="preserve">Student Git Address: https://github.com/JulDel158/PPIV-Project.git </t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -935,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1868,7 +1871,9 @@
       <c r="D37" s="5">
         <v>1</v>
       </c>
-      <c r="E37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="F37" s="3"/>
       <c r="G37" s="16">
         <f t="shared" si="0"/>
@@ -3222,7 +3227,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added new model (axe1.h) for testing purposes
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25E3DD7-A948-4A89-A3AE-CB61D9988ADB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD14EF29-1612-4602-82E7-26865680668F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -938,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,7 +1064,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1077,7 +1080,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1202,7 +1205,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 30, IF(K4+H4 &gt; 30, 30- H4, K4),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
@@ -1874,10 +1877,12 @@
       <c r="E37" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F37" s="3"/>
+      <c r="F37" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G37" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -3227,7 +3232,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added Grid and grid generator function Row 38 completed
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD14EF29-1612-4602-82E7-26865680668F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE61DFA1-2110-47F1-869D-B212979680EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 30, IF(K4+H4 &gt; 30, 30- H4, K4),0)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
@@ -1903,11 +1903,15 @@
       <c r="D38" s="5">
         <v>1</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="3"/>
+      <c r="E38" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G38" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -3232,7 +3236,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added simple OBJ loader Removed unnecessary duplicate code added Wave_VS.hlsl in anticipation of wave vertex shader (similar to water or a flag)
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE61DFA1-2110-47F1-869D-B212979680EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A53132-3B23-4213-900A-58D92D0A20E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -941,7 +941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
@@ -3236,7 +3236,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added directional light in PixelShader.hlsl
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A53132-3B23-4213-900A-58D92D0A20E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F629E52-6CB1-4123-804F-961D9497991D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1056,15 +1056,19 @@
       <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G67" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1080,7 +1084,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1205,7 +1209,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 30, IF(K4+H4 &gt; 30, 30- H4, K4),0)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
@@ -3236,7 +3240,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Wave_VS.hlsl now modifies y position of vertex to create waves
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F629E52-6CB1-4123-804F-961D9497991D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAB869B-8D2E-41D3-833C-B1F52D3C2F84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 30, IF(K4+H4 &gt; 30, 30- H4, K4),0)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
@@ -1675,11 +1675,15 @@
       <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="3"/>
+      <c r="E28" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G28" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -3240,7 +3244,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Modified PixelShader.hlsl to use texture WARNING: No default texture in place. All objects are currently using the axe texture as a default Non texture shader or default texture needed.
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAB869B-8D2E-41D3-833C-B1F52D3C2F84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCEC2D7-9A0E-4BE4-8069-DC876B5CD496}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 30, IF(K4+H4 &gt; 30, 30- H4, K4),0)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
@@ -1514,11 +1514,15 @@
       <c r="D21" s="5">
         <v>2</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G21" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -3244,7 +3248,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added simple point light logic
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCEC2D7-9A0E-4BE4-8069-DC876B5CD496}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F4DB29-8162-47B1-B477-6A0B658DD80A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -942,7 +942,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1100,11 +1100,15 @@
       <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>26</v>
@@ -1170,11 +1174,15 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>22</v>
@@ -1209,7 +1217,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 30, IF(K4+H4 &gt; 30, 30- H4, K4),0)</f>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
@@ -3248,7 +3256,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Updated rubric Row 39 Completed
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F4DB29-8162-47B1-B477-6A0B658DD80A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBBA4CA-84E6-4F96-A062-E92FD4A99241}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 30, IF(K4+H4 &gt; 30, 30- H4, K4),0)</f>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
@@ -1952,11 +1952,15 @@
       <c r="D39" s="5">
         <v>4</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="3"/>
+      <c r="E39" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G39" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -3256,7 +3260,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Updated PlaneGrid and Wave_VS.hlsl Wave_VS now generates a wave similar to water/flag (in progress)
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBBA4CA-84E6-4F96-A062-E92FD4A99241}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69089531-E7B1-46F3-84F5-F43D7903CEC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -942,7 +942,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1080,11 +1080,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1145,7 +1145,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 30, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 30,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 30,0)</f>
@@ -1217,11 +1217,11 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 30, IF(K4+H4 &gt; 30, 30- H4, K4),0)</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 30, IF(I10+J4 &gt; 30, 30- J4, I10),0)</f>
@@ -1282,7 +1282,7 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 30 &gt; 0, K4+H4 - 30, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 30 &gt; 0, H10+I4 - 30, 0)</f>
@@ -2131,11 +2131,15 @@
       <c r="D46" s="5">
         <v>2</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="3"/>
+      <c r="E46" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G46" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
@@ -3107,7 +3111,9 @@
       <c r="B91" s="6">
         <v>2</v>
       </c>
-      <c r="C91" s="3"/>
+      <c r="C91" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
@@ -3125,7 +3131,9 @@
       <c r="B92" s="6">
         <v>1</v>
       </c>
-      <c r="C92" s="3"/>
+      <c r="C92" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="5"/>

</xml_diff>

<commit_message>
Updated the rubic and also included the needed pixel shader
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69089531-E7B1-46F3-84F5-F43D7903CEC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0593E3-80F1-4155-99BE-AFCF857655B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -941,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,7 +1075,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1084,7 +1087,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1221,7 +1224,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 30, IF(I10+J4 &gt; 30, 30- J4, I10),0)</f>
@@ -1981,11 +1984,15 @@
       <c r="D40" s="5">
         <v>3</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="3"/>
+      <c r="E40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G40" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -3268,7 +3275,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Update pixel shader in preparation for specular reflection Moving point light dynamically
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0593E3-80F1-4155-99BE-AFCF857655B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC43D0A-6C7C-4F1F-B4D7-02DED6FAE4FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -345,6 +345,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>https://catlikecoding.com/unity/tutorials/flow/waves/ wave tutorial by Jasper Flick</t>
   </si>
 </sst>
 </file>
@@ -944,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,7 +1078,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1087,7 +1090,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1224,7 +1227,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 30, IF(I10+J4 &gt; 30, 30- J4, I10),0)</f>
@@ -1246,11 +1249,15 @@
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>25</v>
@@ -3185,7 +3192,9 @@
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A96" s="12"/>
+      <c r="A96" s="12" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="12"/>

</xml_diff>

<commit_message>
Added spotlight update all light code into functions on shaders constant buffers slightly changed
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC43D0A-6C7C-4F1F-B4D7-02DED6FAE4FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68EAC27-9891-407A-BE26-B931892B0911}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1143,11 +1143,15 @@
       <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 30, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 30,0)</f>
@@ -1227,7 +1231,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 30, IF(I10+J4 &gt; 30, 30- J4, I10),0)</f>
@@ -1418,7 +1422,9 @@
       <c r="D15" s="5">
         <v>2</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="16">
         <f t="shared" si="0"/>
@@ -3284,7 +3290,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
small changes on pixel shaders and constant buffer
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68EAC27-9891-407A-BE26-B931892B0911}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A487C9-1799-4363-AB76-4E4072AA346C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 30, IF(I10+J4 &gt; 30, 30- J4, I10),0)</f>
@@ -2394,11 +2394,15 @@
       <c r="D57" s="5">
         <v>2</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="3"/>
+      <c r="E57" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G57" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -2522,11 +2526,15 @@
       <c r="D63" s="5">
         <v>2</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="3"/>
+      <c r="E63" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G63" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
@@ -3134,7 +3142,9 @@
       <c r="C91" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -3154,7 +3164,9 @@
       <c r="C92" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D92" s="3"/>
+      <c r="D92" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="E92" s="3"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
@@ -3290,7 +3302,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Camera movement calculations fixed, camera now moves as expected from input
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448D2603-9040-4B80-839D-868EF260E605}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DEDA30-008E-4ADA-AC04-261E4D7E6CC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 30, IF(I10+J4 &gt; 30, 30- J4, I10),0)</f>
@@ -1619,11 +1619,15 @@
       <c r="D24" s="5">
         <v>3</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G24" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>

</xml_diff>

<commit_message>
Updated rubric for milestone 2
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08D7085-E20F-4FFA-B793-47A8D7771FC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DC05E9-F073-48AD-9A6F-2B1D9C632C6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -947,25 +947,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="C27" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="106.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="106.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1"/>
-    <col min="8" max="9" width="25.85546875" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" customWidth="1"/>
+    <col min="4" max="6" width="25.44140625" customWidth="1"/>
+    <col min="7" max="7" width="25.5546875" customWidth="1"/>
+    <col min="8" max="9" width="25.88671875" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" customWidth="1"/>
+    <col min="11" max="11" width="24.44140625" customWidth="1"/>
+    <col min="12" max="12" width="24.109375" customWidth="1"/>
+    <col min="13" max="14" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>100</v>
       </c>
@@ -981,7 +981,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>101</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>96</v>
       </c>
@@ -1086,14 +1086,14 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>92</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>71</v>
       </c>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 30, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 30,0)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 30,0)</f>
@@ -1171,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>38</v>
       </c>
@@ -1206,7 +1206,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>39</v>
       </c>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 30, IF(I10+J4 &gt; 30, 30- J4, I10),0)</f>
@@ -1240,7 +1240,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>40</v>
       </c>
@@ -1275,7 +1275,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>41</v>
       </c>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 30 &gt; 0, K4+H4 - 30, 0)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 30 &gt; 0, H10+I4 - 30, 0)</f>
@@ -1309,7 +1309,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>49</v>
       </c>
@@ -1334,7 +1334,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>56</v>
       </c>
@@ -1359,7 +1359,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>74</v>
       </c>
@@ -1384,7 +1384,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>75</v>
       </c>
@@ -1409,7 +1409,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>45</v>
       </c>
@@ -1438,7 +1438,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1455,7 +1455,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>51</v>
       </c>
@@ -1474,7 +1474,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1491,7 +1491,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1508,7 +1508,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>9</v>
       </c>
@@ -1527,7 +1527,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>36</v>
       </c>
@@ -1556,7 +1556,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>50</v>
       </c>
@@ -1581,7 +1581,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>37</v>
       </c>
@@ -1606,7 +1606,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>35</v>
       </c>
@@ -1635,7 +1635,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>76</v>
       </c>
@@ -1660,7 +1660,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1677,7 +1677,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>72</v>
       </c>
@@ -1696,7 +1696,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>77</v>
       </c>
@@ -1725,7 +1725,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>64</v>
       </c>
@@ -1750,7 +1750,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>66</v>
       </c>
@@ -1775,7 +1775,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>65</v>
       </c>
@@ -1800,7 +1800,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>67</v>
       </c>
@@ -1825,7 +1825,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>68</v>
       </c>
@@ -1850,7 +1850,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1867,7 +1867,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1884,7 +1884,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>52</v>
       </c>
@@ -1903,7 +1903,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
         <v>97</v>
       </c>
@@ -1932,7 +1932,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="24" t="s">
         <v>78</v>
       </c>
@@ -1961,7 +1961,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>93</v>
       </c>
@@ -1990,7 +1990,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>91</v>
       </c>
@@ -2019,7 +2019,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>44</v>
       </c>
@@ -2044,7 +2044,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>32</v>
       </c>
@@ -2069,7 +2069,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>33</v>
       </c>
@@ -2094,7 +2094,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>53</v>
       </c>
@@ -2119,7 +2119,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>34</v>
       </c>
@@ -2144,7 +2144,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
         <v>69</v>
       </c>
@@ -2173,7 +2173,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="22"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2190,7 +2190,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2207,7 +2207,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>7</v>
       </c>
@@ -2226,7 +2226,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
         <v>73</v>
       </c>
@@ -2251,7 +2251,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>46</v>
       </c>
@@ -2276,7 +2276,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>54</v>
       </c>
@@ -2301,7 +2301,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>70</v>
       </c>
@@ -2326,7 +2326,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="8"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2343,7 +2343,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
         <v>6</v>
       </c>
@@ -2362,7 +2362,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>79</v>
       </c>
@@ -2387,7 +2387,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>63</v>
       </c>
@@ -2403,12 +2403,10 @@
       <c r="E57" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F57" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="F57" s="3"/>
       <c r="G57" s="16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -2416,7 +2414,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
         <v>98</v>
       </c>
@@ -2441,7 +2439,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>47</v>
       </c>
@@ -2466,7 +2464,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="8"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2483,7 +2481,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="8"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2500,7 +2498,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>5</v>
       </c>
@@ -2519,7 +2517,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>99</v>
       </c>
@@ -2548,7 +2546,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
         <v>94</v>
       </c>
@@ -2562,7 +2560,7 @@
         <v>1</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>103</v>
@@ -2577,7 +2575,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
         <v>81</v>
       </c>
@@ -2602,7 +2600,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="20" t="s">
         <v>57</v>
       </c>
@@ -2616,7 +2614,7 @@
         <v>1</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>103</v>
@@ -2631,7 +2629,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="21" t="s">
         <v>55</v>
       </c>
@@ -2656,7 +2654,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
         <v>48</v>
       </c>
@@ -2681,7 +2679,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="8"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2698,7 +2696,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="8"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2715,7 +2713,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>4</v>
       </c>
@@ -2734,7 +2732,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
         <v>84</v>
       </c>
@@ -2759,7 +2757,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
         <v>90</v>
       </c>
@@ -2784,7 +2782,7 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
         <v>85</v>
       </c>
@@ -2809,7 +2807,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
         <v>87</v>
       </c>
@@ -2834,7 +2832,7 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
         <v>86</v>
       </c>
@@ -2859,7 +2857,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
         <v>88</v>
       </c>
@@ -2884,7 +2882,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
         <v>89</v>
       </c>
@@ -2909,7 +2907,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="11"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
@@ -2926,7 +2924,7 @@
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="11"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
@@ -2943,7 +2941,7 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
         <v>83</v>
       </c>
@@ -2962,7 +2960,7 @@
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
         <v>61</v>
       </c>
@@ -2983,7 +2981,7 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
         <v>62</v>
       </c>
@@ -3004,7 +3002,7 @@
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="11" t="s">
         <v>82</v>
       </c>
@@ -3025,7 +3023,7 @@
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="11" t="s">
         <v>59</v>
       </c>
@@ -3046,7 +3044,7 @@
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="11" t="s">
         <v>58</v>
       </c>
@@ -3067,7 +3065,7 @@
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="11" t="s">
         <v>60</v>
       </c>
@@ -3088,7 +3086,7 @@
       <c r="K87" s="5"/>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="8"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3105,7 +3103,7 @@
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="8"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3122,7 +3120,7 @@
       <c r="K89" s="5"/>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
         <v>30</v>
       </c>
@@ -3146,7 +3144,7 @@
       <c r="K90" s="6"/>
       <c r="L90" s="5"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="10" t="s">
         <v>17</v>
       </c>
@@ -3168,7 +3166,7 @@
       <c r="K91" s="6"/>
       <c r="L91" s="5"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
         <v>28</v>
       </c>
@@ -3190,7 +3188,7 @@
       <c r="K92" s="6"/>
       <c r="L92" s="5"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="11"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -3204,7 +3202,7 @@
       <c r="K93" s="6"/>
       <c r="L93" s="5"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="11"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
@@ -3218,80 +3216,80 @@
       <c r="K94" s="5"/>
       <c r="L94" s="5"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="12"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="12"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="12"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="12"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="12"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="12"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="12"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="12"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="12"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="12"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="12"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="12"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="12"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="12"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="12"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="12"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="12"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="12"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="12"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="12"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="12"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="13"/>
     </row>
   </sheetData>
@@ -3386,7 +3384,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3403,7 +3401,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Adding Island terrain for theme
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9220C8EE-26ED-44A8-B7EC-59BF239FAD4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A9E741-F5CB-4C07-ABC5-249A57F78F7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="108">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -348,6 +348,12 @@
   </si>
   <si>
     <t>https://catlikecoding.com/unity/tutorials/flow/waves/ wave tutorial by Jasper Flick</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>https://www.cgtrader.com/free-3d-models/exterior/landscape/coconut-tree-island-low-poly</t>
   </si>
 </sst>
 </file>
@@ -947,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1074,7 +1080,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1082,15 +1088,15 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 30, 30, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1107,7 +1113,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>103</v>
@@ -1155,7 +1161,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 30, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 30,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 30, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 30,0)</f>
@@ -1227,15 +1233,15 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 30, IF(K4+H4 &gt; 30, 30- H4, K4),0)</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 30, IF(H10+I4 &gt; 30, 30- I4, H10),0)</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 30, IF(I10+J4 &gt; 30, 30- J4, I10),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1296,7 +1302,7 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 30 &gt; 0, K4+H4 - 30, 0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 30 &gt; 0, H10+I4 - 30, 0)</f>
@@ -1425,12 +1431,10 @@
       <c r="E15" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="F15" s="3"/>
       <c r="G15" s="16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -2032,7 +2036,9 @@
       <c r="D41" s="5">
         <v>3</v>
       </c>
-      <c r="E41" s="2"/>
+      <c r="E41" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="F41" s="3"/>
       <c r="G41" s="16">
         <f t="shared" si="0"/>
@@ -2531,7 +2537,7 @@
         <v>2</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>103</v>
@@ -2642,7 +2648,9 @@
       <c r="D67" s="5">
         <v>4</v>
       </c>
-      <c r="E67" s="2"/>
+      <c r="E67" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="F67" s="3"/>
       <c r="G67" s="16">
         <f t="shared" si="0"/>
@@ -3032,7 +3040,9 @@
       <c r="D85" s="5">
         <v>5</v>
       </c>
-      <c r="E85" s="2"/>
+      <c r="E85" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="F85" s="3"/>
       <c r="G85" s="16">
         <f t="shared" si="1"/>
@@ -3227,7 +3237,9 @@
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="12"/>
+      <c r="A97" s="12" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="12"/>
@@ -3314,7 +3326,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
removing unused assets adding assets references into rubric
</commit_message>
<xml_diff>
--- a/Dev IV Group Project Rubric.xlsx
+++ b/Dev IV Group Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B77E477-3524-44D1-83AA-9380B75081D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D181FF9-25D7-49C1-89AB-C0B4D1FC584E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="116">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -375,13 +375,16 @@
   </si>
   <si>
     <t>https://opengameart.org/content/space-skyboxes-0</t>
+  </si>
+  <si>
+    <t>https://www.solarsystemscope.com/textures/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,6 +430,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -551,7 +560,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -631,6 +640,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -974,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3308,7 +3320,9 @@
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" s="12"/>
+      <c r="A105" s="26" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="12"/>
@@ -3371,7 +3385,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>